<commit_message>
Attempting to reduce word count.
</commit_message>
<xml_diff>
--- a/docs/report/attached_documents/user_feedback.xlsx
+++ b/docs/report/attached_documents/user_feedback.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\education\roehampton_university\2022-2023\final_year_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD0A824-315B-42B2-9C2D-2EF7E8F1D497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2459EBB-134B-4D79-A4FA-5BD06C9EA94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6870" yWindow="675" windowWidth="18420" windowHeight="12420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>User</t>
   </si>
@@ -94,6 +106,36 @@
   </si>
   <si>
     <t>Not completed</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Votes</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Lighting</t>
+  </si>
+  <si>
+    <t>Encryption</t>
   </si>
 </sst>
 </file>
@@ -207,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -225,6 +267,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -241,6 +284,1890 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Ease</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of Use</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$3:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Tyler</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Adam</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tom</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Trevor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bogdan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FCE2-425B-A772-261EAE4C3A1F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1267483904"/>
+        <c:axId val="1264789200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1267483904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1264789200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1264789200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1267483904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Votes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$22:$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Performance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>User Interface</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Settings</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lighting</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Encryption</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$22:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F770-4256-A134-A52A9CC0223A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46748AA1-3287-9C11-5B03-C18B884EBAB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>261768</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>184674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>562086</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>184674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6038C270-C348-1543-4DF8-A25596609D8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -508,7 +2435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -778,4 +2705,126 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82D9E3C-61F1-48A4-A9AE-F1C2111A9D6B}">
+  <dimension ref="B2:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>AVERAGE(C3:C7)</f>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>